<commit_message>
Working version with MA data (1 auth, 2 sections)
</commit_message>
<xml_diff>
--- a/data for upload/Question.xlsx
+++ b/data for upload/Question.xlsx
@@ -5,17 +5,33 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Documents/Coding/1. Render/data_driven_forms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Documents/Coding/1. Render/data_driven_forms/data for upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{12124849-B4CB-F14E-93A7-8134E92C6CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD2BD5C-C347-A547-99F4-5D2EEA877E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15720" xr2:uid="{645198BA-45AB-404C-A743-07DB123742AC}"/>
+    <workbookView xWindow="260" yWindow="6260" windowWidth="27640" windowHeight="15720" xr2:uid="{645198BA-45AB-404C-A743-07DB123742AC}"/>
   </bookViews>
   <sheets>
     <sheet name="screen_questions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">screen_questions!$A$1:$H$9</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1027,7 +1043,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1215,6 +1231,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H9" xr:uid="{ADBEF359-F3AE-B14D-BBC4-1D6026DF12EB}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>